<commit_message>
Added fab note to BoM file; added DFM report
</commit_message>
<xml_diff>
--- a/Bill of Materials/core-bom-v021.xlsx
+++ b/Bill of Materials/core-bom-v021.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11660" yWindow="3140" windowWidth="33020" windowHeight="21620" tabRatio="500"/>
+    <workbookView xWindow="4820" yWindow="2380" windowWidth="33020" windowHeight="21620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
+    <sheet name="Fab Notes for PCB Vendor" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -145,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="179">
   <si>
     <t>Value</t>
   </si>
@@ -617,9 +618,6 @@
     <t>MIC5209-3.3YS</t>
   </si>
   <si>
-    <t>Switch to through-hole version</t>
-  </si>
-  <si>
     <t>Probably fine, but will need to test</t>
   </si>
   <si>
@@ -672,6 +670,33 @@
   </si>
   <si>
     <t>C0603C104K3RACTU</t>
+  </si>
+  <si>
+    <t>CMCUSB-5BFM2G-01-D</t>
+  </si>
+  <si>
+    <t>Need price quote? Might be super expensive.</t>
+  </si>
+  <si>
+    <t>Fab notes for PCB vendor</t>
+  </si>
+  <si>
+    <t>Specified for 7628 single sided 7 mil prepreg</t>
+  </si>
+  <si>
+    <t>Er (dielectric constant) between 4.5 and 4.7</t>
+  </si>
+  <si>
+    <t>Board thickness of 1.6mm</t>
+  </si>
+  <si>
+    <t>Distance of 0.014"/356um between layers 1 and 2</t>
+  </si>
+  <si>
+    <t>Target impedance of 50 ohms on RF net (see drawing)</t>
+  </si>
+  <si>
+    <t>Plug and tent all vias on the top side of the board</t>
   </si>
 </sst>
 </file>
@@ -863,7 +888,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="148">
+  <cellStyleXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1012,8 +1037,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1063,9 +1092,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="123" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="123" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="124" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1089,6 +1115,18 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="123" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="131" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="123" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1104,20 +1142,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="123" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="131" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="123" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="131" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="148">
+  <cellStyles count="152">
     <cellStyle name="Bad" xfId="124" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1191,6 +1221,8 @@
     <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="123" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1264,6 +1296,8 @@
     <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="131" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1596,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:N45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1622,56 +1656,56 @@
     <row r="3" spans="2:14">
       <c r="B3" s="6"/>
       <c r="C3" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="2:14">
       <c r="B4" s="7"/>
       <c r="C4" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="2:14">
       <c r="B5" s="8"/>
       <c r="C5" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="2:14">
       <c r="B6"/>
-      <c r="C6" s="26"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="27">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="B8" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="28">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14">
-      <c r="B8" s="34" t="s">
+      <c r="C8" s="37"/>
+      <c r="D8" s="27">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="28">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14">
-      <c r="B9" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="29">
+      <c r="C9" s="38"/>
+      <c r="D9" s="28">
         <f>SUM(D7:D8)</f>
         <v>13200</v>
       </c>
     </row>
     <row r="10" spans="2:14">
-      <c r="B10" s="27"/>
-      <c r="C10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="25"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="2" t="s">
@@ -1696,22 +1730,22 @@
         <v>142</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J12" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="N12" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="13" spans="2:14">
@@ -1721,18 +1755,18 @@
       <c r="C13" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="11" t="s">
         <v>143</v>
       </c>
       <c r="J13" s="11"/>
-      <c r="K13" s="30">
+      <c r="K13" s="29">
         <f>B13*$D$9</f>
         <v>13200</v>
       </c>
@@ -1764,7 +1798,7 @@
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
-      <c r="K14" s="30">
+      <c r="K14" s="29">
         <f>B14*$D$7</f>
         <v>12000</v>
       </c>
@@ -1798,7 +1832,7 @@
         <v>144</v>
       </c>
       <c r="J15" s="11"/>
-      <c r="K15" s="30">
+      <c r="K15" s="29">
         <f t="shared" ref="K15:K45" si="0">B15*$D$9</f>
         <v>26400</v>
       </c>
@@ -1807,7 +1841,7 @@
       <c r="N15" s="11"/>
     </row>
     <row r="16" spans="2:14">
-      <c r="B16" s="36">
+      <c r="B16" s="30">
         <v>1</v>
       </c>
       <c r="C16" s="15" t="s">
@@ -1822,15 +1856,15 @@
       <c r="F16" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="G16" s="37" t="s">
+      <c r="G16" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="H16" s="31" t="s">
         <v>169</v>
-      </c>
-      <c r="H16" s="37" t="s">
-        <v>170</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
-      <c r="K16" s="30">
+      <c r="K16" s="29">
         <f>B16*$D$9</f>
         <v>13200</v>
       </c>
@@ -1854,15 +1888,17 @@
       <c r="F17" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="I17" s="11"/>
+      <c r="H17" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>171</v>
+      </c>
       <c r="J17" s="11"/>
-      <c r="K17" s="30">
+      <c r="K17" s="29">
         <f>D8+D7</f>
         <v>13200</v>
       </c>
@@ -1871,7 +1907,7 @@
       <c r="N17" s="11"/>
     </row>
     <row r="18" spans="2:14">
-      <c r="B18" s="36">
+      <c r="B18" s="30">
         <v>4</v>
       </c>
       <c r="C18" s="18" t="s">
@@ -1894,7 +1930,7 @@
       </c>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="30">
+      <c r="K18" s="29">
         <f t="shared" si="0"/>
         <v>52800</v>
       </c>
@@ -1926,7 +1962,7 @@
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="30">
+      <c r="K19" s="29">
         <f t="shared" si="0"/>
         <v>92400</v>
       </c>
@@ -1950,15 +1986,17 @@
       <c r="F20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G20" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="I20" s="11"/>
+      <c r="I20" s="11" t="s">
+        <v>171</v>
+      </c>
       <c r="J20" s="11"/>
-      <c r="K20" s="30">
+      <c r="K20" s="29">
         <f>B20*$D$7</f>
         <v>12000</v>
       </c>
@@ -1967,7 +2005,7 @@
       <c r="N20" s="11"/>
     </row>
     <row r="21" spans="2:14">
-      <c r="B21" s="36">
+      <c r="B21" s="30">
         <v>2</v>
       </c>
       <c r="C21" s="18" t="s">
@@ -1990,7 +2028,7 @@
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="30">
+      <c r="K21" s="29">
         <f t="shared" si="0"/>
         <v>26400</v>
       </c>
@@ -2022,7 +2060,7 @@
       </c>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
-      <c r="K22" s="30">
+      <c r="K22" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2056,7 +2094,7 @@
         <v>150</v>
       </c>
       <c r="J23" s="11"/>
-      <c r="K23" s="30">
+      <c r="K23" s="29">
         <f t="shared" si="0"/>
         <v>26400</v>
       </c>
@@ -2088,7 +2126,7 @@
       </c>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
-      <c r="K24" s="30">
+      <c r="K24" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2120,7 +2158,7 @@
       </c>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
-      <c r="K25" s="30">
+      <c r="K25" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2152,7 +2190,7 @@
       </c>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
-      <c r="K26" s="30">
+      <c r="K26" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2184,7 +2222,7 @@
       </c>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
-      <c r="K27" s="30">
+      <c r="K27" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2216,7 +2254,7 @@
       </c>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
-      <c r="K28" s="30">
+      <c r="K28" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2248,7 +2286,7 @@
       </c>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
-      <c r="K29" s="30">
+      <c r="K29" s="29">
         <f t="shared" si="0"/>
         <v>26400</v>
       </c>
@@ -2280,7 +2318,7 @@
       </c>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
-      <c r="K30" s="30">
+      <c r="K30" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2312,7 +2350,7 @@
       </c>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
-      <c r="K31" s="30">
+      <c r="K31" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2344,7 +2382,7 @@
       </c>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
-      <c r="K32" s="30">
+      <c r="K32" s="29">
         <f t="shared" si="0"/>
         <v>26400</v>
       </c>
@@ -2376,7 +2414,7 @@
       </c>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
-      <c r="K33" s="30">
+      <c r="K33" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2408,7 +2446,7 @@
       </c>
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
-      <c r="K34" s="30">
+      <c r="K34" s="29">
         <f t="shared" si="0"/>
         <v>26400</v>
       </c>
@@ -2440,7 +2478,7 @@
       </c>
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
-      <c r="K35" s="30">
+      <c r="K35" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2464,15 +2502,15 @@
       <c r="F36" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="21" t="s">
+      <c r="G36" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="H36" s="21" t="s">
+      <c r="H36" s="15" t="s">
         <v>151</v>
       </c>
       <c r="I36" s="11"/>
       <c r="J36" s="11"/>
-      <c r="K36" s="30">
+      <c r="K36" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2504,7 +2542,7 @@
       </c>
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
-      <c r="K37" s="30">
+      <c r="K37" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2536,7 +2574,7 @@
       </c>
       <c r="I38" s="11"/>
       <c r="J38" s="11"/>
-      <c r="K38" s="30">
+      <c r="K38" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2548,25 +2586,25 @@
       <c r="B39" s="14">
         <v>1</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D39" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22" t="s">
+      <c r="E39" s="21"/>
+      <c r="F39" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="G39" s="22" t="s">
+      <c r="G39" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="H39" s="22" t="s">
+      <c r="H39" s="21" t="s">
         <v>126</v>
       </c>
       <c r="I39" s="11"/>
       <c r="J39" s="11"/>
-      <c r="K39" s="30">
+      <c r="K39" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2590,13 +2628,15 @@
       <c r="F40" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="11" t="s">
-        <v>152</v>
-      </c>
+      <c r="G40" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="I40" s="11"/>
       <c r="J40" s="11"/>
-      <c r="K40" s="30">
+      <c r="K40" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2627,10 +2667,10 @@
         <v>130</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J41" s="11"/>
-      <c r="K41" s="30">
+      <c r="K41" s="29">
         <f>B41*$D$8</f>
         <v>1200</v>
       </c>
@@ -2657,10 +2697,10 @@
       <c r="G42" s="17"/>
       <c r="H42" s="17"/>
       <c r="I42" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J42" s="11"/>
-      <c r="K42" s="30">
+      <c r="K42" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2685,12 +2725,12 @@
         <v>45</v>
       </c>
       <c r="G43" s="17"/>
-      <c r="H43" s="24"/>
+      <c r="H43" s="23"/>
       <c r="I43" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J43" s="11"/>
-      <c r="K43" s="30">
+      <c r="K43" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2711,10 +2751,10 @@
       <c r="E44" s="19"/>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
-      <c r="H44" s="25"/>
+      <c r="H44" s="24"/>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
-      <c r="K44" s="30">
+      <c r="K44" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2733,10 +2773,10 @@
       <c r="E45" s="19"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
-      <c r="H45" s="25"/>
+      <c r="H45" s="24"/>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
-      <c r="K45" s="30">
+      <c r="K45" s="29">
         <f t="shared" si="0"/>
         <v>13200</v>
       </c>
@@ -2762,4 +2802,64 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:B8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" style="26" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" s="40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" s="26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" s="26" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated all supplementary files
</commit_message>
<xml_diff>
--- a/Bill of Materials/core-bom-v021.xlsx
+++ b/Bill of Materials/core-bom-v021.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21920" tabRatio="500"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="169">
   <si>
     <t>Device</t>
   </si>
@@ -664,15 +664,6 @@
   </si>
   <si>
     <t>FR4, 1.6mm, 1OZ, Electroless Nickel Immersion Gold, White Solder Mask, Black Silkscreen</t>
-  </si>
-  <si>
-    <t>Core - Chip Antenna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Core - u.FL </t>
-  </si>
-  <si>
-    <t>TOTAL</t>
   </si>
   <si>
     <t>LAST UPDATED</t>
@@ -686,7 +677,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -748,12 +739,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -1142,7 +1127,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1160,19 +1145,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="123" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1194,9 +1166,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="123" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1219,17 +1188,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="124" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="123" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="123" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="287">
@@ -1848,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J51"/>
+  <dimension ref="B1:J46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1875,11 +1847,11 @@
       <c r="D1" s="8"/>
     </row>
     <row r="2" spans="2:10" ht="16" thickBot="1">
-      <c r="B2" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="39">
+      <c r="B2" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="32">
         <v>41473</v>
       </c>
     </row>
@@ -1889,876 +1861,905 @@
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="10">
-        <v>10200</v>
+      <c r="B4" s="30" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="33">
+        <v>7</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="33">
+        <v>4</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="33">
+        <v>2</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="12">
+        <v>2</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="12">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="30">
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="10">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="11">
-        <f>SUM(D4:D5)</f>
-        <v>13200</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="36" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="2" t="s">
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="33">
+        <v>1</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="33">
+        <v>1</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="33">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="33">
+        <v>1</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="33">
+        <v>1</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="33">
+        <v>1</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="12">
+        <v>2</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="33">
+        <v>1</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="33">
+        <v>1</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="33">
+        <v>2</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="33">
+        <v>2</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="33">
+        <v>2</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="33">
+        <v>1</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="33">
+        <v>1</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" s="33">
+        <v>1</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="33">
+        <v>1</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="33">
+        <v>1</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="33">
+        <v>1</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="33">
+        <v>2</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="33">
+        <v>1</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="33">
+        <v>1</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="33">
+        <v>1</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="33">
+        <v>1</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" s="19"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="26"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="8"/>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H39" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I39" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J39" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="23">
+    <row r="40" spans="2:10">
+      <c r="B40" s="12">
         <v>1</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="41">
-        <v>7</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="41">
-        <v>4</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="41">
-        <v>2</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="B15" s="17">
-        <v>2</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" s="17">
+      <c r="C40" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="12">
         <v>1</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="30">
-      <c r="B17" s="14">
-        <v>1</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>171</v>
-      </c>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="41">
-        <v>1</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="2:10">
-      <c r="B19" s="41">
-        <v>1</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="41">
-        <v>1</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="41">
-        <v>1</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="I21" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="41">
-        <v>1</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="41">
-        <v>1</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="17">
-        <v>2</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="H24" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="2:10">
-      <c r="B25" s="41">
-        <v>1</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="I25" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="2:10">
-      <c r="B26" s="41">
-        <v>1</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="2:10">
-      <c r="B27" s="41">
-        <v>2</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I27" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="2:10">
-      <c r="B28" s="41">
-        <v>2</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I28" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="2:10">
-      <c r="B29" s="41">
-        <v>2</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H29" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I29" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="2:10">
-      <c r="B30" s="41">
-        <v>1</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="2:10">
-      <c r="B31" s="41">
-        <v>1</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I31" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="2:10">
-      <c r="B32" s="41">
-        <v>1</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I32" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="2:10">
-      <c r="B33" s="41">
-        <v>1</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="I33" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="J33" s="5"/>
-    </row>
-    <row r="34" spans="2:10">
-      <c r="B34" s="41">
-        <v>1</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="I34" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="2:10">
-      <c r="B35" s="41">
-        <v>1</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="2:10">
-      <c r="B36" s="41">
-        <v>2</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H36" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="I36" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="2:10">
-      <c r="B37" s="41">
-        <v>1</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="H37" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="I37" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="2:10">
-      <c r="B38" s="41">
-        <v>1</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="H38" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I38" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="2:10">
-      <c r="B39" s="41">
-        <v>1</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D39" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="28" t="s">
+      <c r="C41" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="I39" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="2:10">
-      <c r="B40" s="41">
-        <v>1</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="G40" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="H40" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="I40" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="2:10">
-      <c r="B41" s="41">
-        <v>1</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="I41" s="18" t="s">
-        <v>135</v>
-      </c>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="10"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="2:10">
-      <c r="B42" s="32"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="8"/>
-    </row>
     <row r="43" spans="2:10">
-      <c r="B43" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="C43" s="33"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="8"/>
+      <c r="B43" s="4" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="44" spans="2:10">
       <c r="B44" s="2" t="s">
@@ -2790,119 +2791,44 @@
       </c>
     </row>
     <row r="45" spans="2:10">
-      <c r="B45" s="17">
+      <c r="B45" s="12">
         <v>1</v>
       </c>
-      <c r="C45" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>158</v>
+      <c r="C45" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>164</v>
       </c>
       <c r="E45" s="5"/>
-      <c r="F45" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="15"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
     <row r="46" spans="2:10">
-      <c r="B46" s="17">
+      <c r="B46" s="12">
         <v>1</v>
       </c>
-      <c r="C46" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="48" spans="2:10">
-      <c r="B48" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10">
-      <c r="B49" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10">
-      <c r="B50" s="17">
-        <v>1</v>
-      </c>
-      <c r="C50" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="2:10">
-      <c r="B51" s="17">
-        <v>1</v>
-      </c>
-      <c r="C51" s="31" t="s">
+      <c r="C46" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="31"/>
-      <c r="J51" s="31"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
     </row>
   </sheetData>
   <sortState ref="B9:J38">
     <sortCondition ref="C9:C38"/>
   </sortState>
-  <mergeCells count="5">
-    <mergeCell ref="D11:I11"/>
+  <mergeCells count="2">
+    <mergeCell ref="D6:I6"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated Core BOM and Stencils
</commit_message>
<xml_diff>
--- a/Bill of Materials/core-bom-v021.xlsx
+++ b/Bill of Materials/core-bom-v021.xlsx
@@ -682,7 +682,7 @@
     <t>47K, 1/10W, 5%</t>
   </si>
   <si>
-    <t>CRCW060322R0JNEA</t>
+    <t>RC0603JR-0722RL</t>
   </si>
 </sst>
 </file>
@@ -850,7 +850,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="295">
+  <cellStyleXfs count="301">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -976,6 +976,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1225,7 +1231,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="295">
+  <cellStyles count="301">
     <cellStyle name="Bad" xfId="124" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1373,6 +1379,9 @@
     <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="123" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1520,6 +1529,9 @@
     <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1852,7 +1864,7 @@
   <dimension ref="B1:J46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1881,6 +1893,7 @@
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="32">
+        <f ca="1">TODAY()</f>
         <v>41479</v>
       </c>
     </row>
@@ -2376,7 +2389,7 @@
         <v>34</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>174</v>

</xml_diff>